<commit_message>
Sample filtering for missing diagnosis and body site information
</commit_message>
<xml_diff>
--- a/data/table1/table1.xlsx
+++ b/data/table1/table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siyuan/Dropbox (Huttenhower Lab)/ibd_paper/data/table1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEEB8FF-C15B-2644-B7C0-CDFC4194C87E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66B7197-DC5F-4E43-8BCC-EB9300E93340}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38660" yWindow="4300" windowWidth="28040" windowHeight="17440" xr2:uid="{B7F1A3C2-2E6F-6F40-A0D1-2A7A1AE215CF}"/>
+    <workbookView xWindow="41960" yWindow="7680" windowWidth="28040" windowHeight="17440" xr2:uid="{B7F1A3C2-2E6F-6F40-A0D1-2A7A1AE215CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>BIDMC-FMT</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Study</t>
   </si>
   <si>
-    <t>Column3</t>
-  </si>
-  <si>
     <t>Column4</t>
   </si>
   <si>
@@ -142,6 +139,21 @@
   </si>
   <si>
     <t>baseline</t>
+  </si>
+  <si>
+    <t>are samples baseline or???</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>No treatment</t>
+  </si>
+  <si>
+    <t>Longitudinal</t>
+  </si>
+  <si>
+    <t>Yes according to paper. Samples before and after FMT</t>
   </si>
 </sst>
 </file>
@@ -219,14 +231,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2DF00EF8-90C1-5E48-A20D-21B5BE379B58}" name="Table1" displayName="Table1" ref="A1:U25" totalsRowShown="0">
-  <autoFilter ref="A1:U25" xr:uid="{2BCC7F96-7412-5B47-809D-4AD825C9E7C0}"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2DF00EF8-90C1-5E48-A20D-21B5BE379B58}" name="Table1" displayName="Table1" ref="A1:V25" totalsRowShown="0">
+  <autoFilter ref="A1:V25" xr:uid="{2BCC7F96-7412-5B47-809D-4AD825C9E7C0}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{966C0E73-DD1C-BE4E-A65C-BA3D57E5FE80}" name="Study"/>
     <tableColumn id="2" xr3:uid="{926628AE-2DD7-ED4C-BFDE-FECACE21A354}" name="PMID"/>
     <tableColumn id="3" xr3:uid="{6F41230F-3407-8748-AD21-34A88E3E6C46}" name="n"/>
+    <tableColumn id="22" xr3:uid="{9E638DB6-4B9A-6C43-9FAB-613C88C0A6E8}" name="Longitudinal"/>
     <tableColumn id="4" xr3:uid="{2AC5AB55-6C3F-AB41-B1B8-F515DD41FC87}" name="Treatment variable"/>
-    <tableColumn id="5" xr3:uid="{D05D7BBE-6E41-624B-8DD3-0F9CC53AA976}" name="Column3"/>
+    <tableColumn id="5" xr3:uid="{D05D7BBE-6E41-624B-8DD3-0F9CC53AA976}" name="Questions"/>
     <tableColumn id="6" xr3:uid="{A5950E67-47D7-3644-BEFF-4B2911FB3906}" name="Column4"/>
     <tableColumn id="7" xr3:uid="{B693AB20-2DDF-C946-AFB8-9C6814F1217E}" name="Column5"/>
     <tableColumn id="8" xr3:uid="{88C8833F-AFCC-8A45-BC08-37F49CD325D8}" name="Column6"/>
@@ -545,208 +558,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BF507E-29B7-E349-97E5-B6D558E8F1E4}">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
-    <col min="12" max="21" width="11.6640625" customWidth="1"/>
+    <col min="13" max="22" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>25</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>27542133</v>
+      </c>
       <c r="C2" s="2">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2">
         <v>428</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>264</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2">
         <v>178</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
         <v>687</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2">
         <v>1614</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2">
         <v>375</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2">
         <v>1212</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2">
         <v>652</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3">
         <v>683</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3">
         <v>118</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2">
         <v>960</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="2">
         <v>138</v>
       </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D15" s="2"/>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>